<commit_message>
#385 Change GDSN language attributes to use language code reference data
</commit_message>
<xml_diff>
--- a/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2020-03-29/8_2_products_trade_items_gdsn_queue.xlsx
+++ b/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2020-03-29/8_2_products_trade_items_gdsn_queue.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="303">
   <si>
     <t xml:space="preserve">sku</t>
   </si>
@@ -520,7 +520,7 @@
     <t xml:space="preserve">Etonogestrel 68 mg/rod, 1 Rod Implant</t>
   </si>
   <si>
-    <t xml:space="preserve">eng</t>
+    <t xml:space="preserve">en</t>
   </si>
   <si>
     <t xml:space="preserve">BASE_UNIT_OR_EACH</t>
@@ -800,9 +800,6 @@
   </si>
   <si>
     <t xml:space="preserve">Levon/Ethiny. 150/30mcg + FE 75mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en</t>
   </si>
   <si>
     <t xml:space="preserve">FALSE</t>
@@ -1035,16 +1032,18 @@
   </sheetPr>
   <dimension ref="A1:EU28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC17" activeCellId="0" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="26" min="1" style="0" width="8.44814814814815"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="24.262962962963"/>
-    <col collapsed="false" hidden="false" max="114" min="28" style="0" width="8.44814814814815"/>
-    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="33.5"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="0" width="8.44814814814815"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="26.2888888888889"/>
+    <col collapsed="false" hidden="false" max="114" min="31" style="0" width="8.44814814814815"/>
+    <col collapsed="false" hidden="false" max="115" min="115" style="0" width="33.5407407407407"/>
     <col collapsed="false" hidden="false" max="1025" min="116" style="0" width="8.44814814814815"/>
   </cols>
   <sheetData>
@@ -1503,7 +1502,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>151</v>
       </c>
@@ -1580,7 +1579,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>169</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>170</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>171</v>
       </c>
@@ -1811,7 +1810,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>172</v>
       </c>
@@ -1888,7 +1887,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>174</v>
       </c>
@@ -1962,7 +1961,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>180</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>185</v>
       </c>
@@ -2149,7 +2148,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>203</v>
       </c>
@@ -2226,7 +2225,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>208</v>
       </c>
@@ -2303,7 +2302,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>209</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>213</v>
       </c>
@@ -2451,7 +2450,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>215</v>
       </c>
@@ -2525,7 +2524,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>216</v>
       </c>
@@ -2599,7 +2598,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>218</v>
       </c>
@@ -2676,7 +2675,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>225</v>
       </c>
@@ -2753,7 +2752,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>229</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>234</v>
       </c>
@@ -2904,7 +2903,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>241</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>243</v>
       </c>
@@ -3043,7 +3042,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>240</v>
       </c>
@@ -3114,7 +3113,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>242</v>
       </c>
@@ -3182,7 +3181,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>248</v>
       </c>
@@ -3306,49 +3305,49 @@
         <v>259</v>
       </c>
       <c r="AE25" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH25" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="AH25" s="1" t="s">
+      <c r="AI25" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="AI25" s="1" t="s">
+      <c r="AN25" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="AN25" s="1" t="s">
+      <c r="AO25" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="AO25" s="1" t="s">
+      <c r="AR25" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="AR25" s="1" t="s">
+      <c r="AS25" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="AS25" s="1" t="s">
+      <c r="AT25" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="AT25" s="1" t="s">
+      <c r="AU25" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AV25" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="AU25" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="AV25" s="1" t="s">
+      <c r="AW25" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="AW25" s="1" t="s">
+      <c r="AX25" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AX25" s="1" t="s">
+      <c r="AY25" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="AY25" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="AZ25" s="1" t="s">
         <v>252</v>
       </c>
       <c r="BA25" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="BF25" s="1" t="s">
         <v>160</v>
@@ -3369,7 +3368,7 @@
         <v>254</v>
       </c>
       <c r="BX25" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="CA25" s="1" t="s">
         <v>160</v>
@@ -3393,7 +3392,7 @@
         <v>255</v>
       </c>
       <c r="CH25" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="CI25" s="1" t="s">
         <v>254</v>
@@ -3402,73 +3401,73 @@
         <v>178</v>
       </c>
       <c r="CP25" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="CQ25" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="CQ25" s="1" t="s">
+      <c r="CR25" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="CS25" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="DE25" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="CR25" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="CS25" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="DE25" s="1" t="s">
+      <c r="DH25" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="DH25" s="1" t="s">
+      <c r="DI25" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="DI25" s="1" t="s">
+      <c r="DJ25" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="DJ25" s="1" t="s">
+      <c r="DK25" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="DK25" s="1" t="s">
+      <c r="DT25" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="DT25" s="1" t="s">
+      <c r="DU25" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="DU25" s="1" t="s">
+      <c r="DV25" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="DW25" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="DV25" s="1" t="s">
+      <c r="DX25" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="DY25" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="DW25" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="DX25" s="1" t="s">
+      <c r="EC25" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="DY25" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="EC25" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="ED25" s="1" t="s">
         <v>164</v>
       </c>
       <c r="EE25" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="EF25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="EG25" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="EF25" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="EG25" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="EH25" s="1" t="s">
-        <v>260</v>
+        <v>166</v>
       </c>
       <c r="EI25" s="1" t="s">
         <v>167</v>
       </c>
       <c r="EJ25" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="EO25" s="1" t="s">
         <v>189</v>
@@ -3482,7 +3481,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>253</v>
@@ -3530,49 +3529,49 @@
         <v>259</v>
       </c>
       <c r="AE26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH26" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="AH26" s="1" t="s">
+      <c r="AI26" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="AI26" s="1" t="s">
+      <c r="AN26" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="AN26" s="1" t="s">
+      <c r="AO26" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="AO26" s="1" t="s">
+      <c r="AR26" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="AR26" s="1" t="s">
+      <c r="AS26" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="AS26" s="1" t="s">
+      <c r="AT26" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="AT26" s="1" t="s">
+      <c r="AU26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AV26" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="AU26" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="AV26" s="1" t="s">
+      <c r="AW26" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="AW26" s="1" t="s">
+      <c r="AX26" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AX26" s="1" t="s">
+      <c r="AY26" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="AY26" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="AZ26" s="1" t="s">
         <v>252</v>
       </c>
       <c r="BA26" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="BF26" s="1" t="s">
         <v>160</v>
@@ -3593,7 +3592,7 @@
         <v>254</v>
       </c>
       <c r="BX26" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="CA26" s="1" t="s">
         <v>160</v>
@@ -3617,7 +3616,7 @@
         <v>255</v>
       </c>
       <c r="CH26" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="CI26" s="1" t="s">
         <v>254</v>
@@ -3626,73 +3625,73 @@
         <v>178</v>
       </c>
       <c r="CP26" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="CQ26" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="CR26" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="CS26" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="DE26" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="DH26" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="CQ26" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="CR26" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="CS26" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="DE26" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="DH26" s="1" t="s">
-        <v>291</v>
-      </c>
       <c r="DI26" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="DJ26" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="DJ26" s="1" t="s">
+      <c r="DK26" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="DK26" s="1" t="s">
+      <c r="DT26" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="DT26" s="1" t="s">
+      <c r="DU26" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="DU26" s="1" t="s">
+      <c r="DV26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="DW26" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="DV26" s="1" t="s">
+      <c r="DX26" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="DY26" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="DW26" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="DX26" s="1" t="s">
+      <c r="EC26" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="DY26" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="EC26" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="ED26" s="1" t="s">
         <v>164</v>
       </c>
       <c r="EE26" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="EF26" s="1" t="s">
         <v>153</v>
       </c>
       <c r="EG26" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="EH26" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EI26" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="EH26" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="EI26" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="EJ26" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="EO26" s="1" t="s">
         <v>189</v>
@@ -3701,12 +3700,12 @@
         <v>190</v>
       </c>
       <c r="ER26" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>253</v>
@@ -3754,49 +3753,49 @@
         <v>259</v>
       </c>
       <c r="AE27" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH27" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="AH27" s="1" t="s">
+      <c r="AI27" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="AI27" s="1" t="s">
+      <c r="AN27" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="AN27" s="1" t="s">
+      <c r="AO27" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="AO27" s="1" t="s">
+      <c r="AR27" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="AR27" s="1" t="s">
+      <c r="AS27" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="AS27" s="1" t="s">
+      <c r="AT27" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="AT27" s="1" t="s">
+      <c r="AU27" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AV27" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="AU27" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="AV27" s="1" t="s">
+      <c r="AW27" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="AW27" s="1" t="s">
+      <c r="AX27" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AX27" s="1" t="s">
+      <c r="AY27" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="AY27" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="AZ27" s="1" t="s">
         <v>252</v>
       </c>
       <c r="BA27" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="BF27" s="1" t="s">
         <v>160</v>
@@ -3817,7 +3816,7 @@
         <v>254</v>
       </c>
       <c r="BX27" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="CA27" s="1" t="s">
         <v>160</v>
@@ -3841,7 +3840,7 @@
         <v>255</v>
       </c>
       <c r="CH27" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="CI27" s="1" t="s">
         <v>254</v>
@@ -3850,73 +3849,73 @@
         <v>178</v>
       </c>
       <c r="CP27" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="CQ27" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="CR27" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="CS27" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="DE27" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="DH27" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="CQ27" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="CR27" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="CS27" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="DE27" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="DH27" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="DI27" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="DJ27" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="DJ27" s="1" t="s">
+      <c r="DK27" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="DK27" s="1" t="s">
+      <c r="DT27" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="DT27" s="1" t="s">
+      <c r="DU27" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="DU27" s="1" t="s">
+      <c r="DV27" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="DW27" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="DV27" s="1" t="s">
+      <c r="DX27" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="DY27" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="DW27" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="DX27" s="1" t="s">
+      <c r="EC27" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="DY27" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="EC27" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="ED27" s="1" t="s">
         <v>164</v>
       </c>
       <c r="EE27" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="EF27" s="1" t="s">
         <v>153</v>
       </c>
       <c r="EG27" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="EH27" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EI27" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="EH27" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="EI27" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="EJ27" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="EO27" s="1" t="s">
         <v>189</v>
@@ -3925,12 +3924,12 @@
         <v>190</v>
       </c>
       <c r="ER27" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>253</v>
@@ -3978,49 +3977,49 @@
         <v>259</v>
       </c>
       <c r="AE28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH28" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="AH28" s="1" t="s">
+      <c r="AI28" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="AI28" s="1" t="s">
+      <c r="AN28" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="AN28" s="1" t="s">
+      <c r="AO28" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="AO28" s="1" t="s">
+      <c r="AR28" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="AR28" s="1" t="s">
+      <c r="AS28" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="AS28" s="1" t="s">
+      <c r="AT28" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="AT28" s="1" t="s">
+      <c r="AU28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AV28" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="AU28" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="AV28" s="1" t="s">
+      <c r="AW28" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="AW28" s="1" t="s">
+      <c r="AX28" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AX28" s="1" t="s">
+      <c r="AY28" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="AY28" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="AZ28" s="1" t="s">
         <v>252</v>
       </c>
       <c r="BA28" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="BF28" s="1" t="s">
         <v>160</v>
@@ -4041,7 +4040,7 @@
         <v>254</v>
       </c>
       <c r="BX28" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="CA28" s="1" t="s">
         <v>160</v>
@@ -4065,7 +4064,7 @@
         <v>255</v>
       </c>
       <c r="CH28" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="CI28" s="1" t="s">
         <v>254</v>
@@ -4074,73 +4073,73 @@
         <v>178</v>
       </c>
       <c r="CP28" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="CQ28" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="CR28" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="CS28" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="DE28" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="DH28" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="CQ28" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="CR28" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="CS28" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="DE28" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="DH28" s="1" t="s">
-        <v>301</v>
-      </c>
       <c r="DI28" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="DJ28" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="DJ28" s="1" t="s">
+      <c r="DK28" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="DK28" s="1" t="s">
+      <c r="DT28" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="DT28" s="1" t="s">
+      <c r="DU28" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="DU28" s="1" t="s">
+      <c r="DV28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="DW28" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="DV28" s="1" t="s">
+      <c r="DX28" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="DY28" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="DW28" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="DX28" s="1" t="s">
+      <c r="EC28" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="DY28" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="EC28" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="ED28" s="1" t="s">
         <v>164</v>
       </c>
       <c r="EE28" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="EF28" s="1" t="s">
         <v>153</v>
       </c>
       <c r="EG28" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="EH28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EI28" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="EH28" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="EI28" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="EJ28" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="EO28" s="1" t="s">
         <v>189</v>
@@ -4149,7 +4148,7 @@
         <v>190</v>
       </c>
       <c r="ER28" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>